<commit_message>
fix schedule dates and item location handling
</commit_message>
<xml_diff>
--- a/life_assist_dm/user_information/권서연.xlsx
+++ b/life_assist_dm/user_information/권서연.xlsx
@@ -959,7 +959,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1188,6 +1188,125 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11:11:40</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Q: 유리컵 냉장고에 있던데? | A: 유리컵을 냉장고에 보관하는 것은 일반적으로 음료를 차갑게 유지하기 위해서입니다. 특히 여름철에 시원한 음료를 마시고 싶을 때 유용할 수 있습니다. 하지만 유리컵은 온도 변화에 따라 깨질 수 있으니 주의해야 합니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11:11:50</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Q: 유리컵 어디있어? | A: 컵은 선반에 있어요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>13:54:35</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Q: 유리컵 어디있어? | A: 컵은 선반에 있어요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>13:56:08</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Q: 유리컵 어디있어? | A: 컵은 선반에 있어요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>14:01:08</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Q: 유리컵 어디있어? | A: 컵은 선반에 있어요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>14:07:16</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Q: 유리컵 어디있어? | A: 컵은 선반에 있어요.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>14:08:55</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Q: 유리컵 어디있어? | A: 컵은 선반에 있어요.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>